<commit_message>
[ADD][DEV] - New version of the ReadMusicXML algorithm name's ReadMusicXMLByInstrument. We now can choose what data are return by instrument. - TO DO next version : return an array of this data to past for Game Engine
</commit_message>
<xml_diff>
--- a/Client/[AudioPipe][19-11-12]DailyScrum1.xlsx
+++ b/Client/[AudioPipe][19-11-12]DailyScrum1.xlsx
@@ -393,7 +393,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.23120607787274455"/>
+          <c:x val="0.23120607787274458"/>
           <c:y val="1.2944983818770227E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -407,7 +407,7 @@
           <c:x val="4.9222842871136832E-2"/>
           <c:y val="0.12821649720969344"/>
           <c:w val="0.81920541983534112"/>
-          <c:h val="0.77895166016869255"/>
+          <c:h val="0.77895166016869277"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -635,23 +635,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="83285888"/>
-        <c:axId val="83287424"/>
+        <c:axId val="81053184"/>
+        <c:axId val="81054720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83285888"/>
+        <c:axId val="81053184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83287424"/>
+        <c:crossAx val="81054720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="83287424"/>
+        <c:axId val="81054720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -659,7 +659,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83285888"/>
+        <c:crossAx val="81053184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -672,7 +672,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -1001,7 +1001,7 @@
   <dimension ref="A1:AJ60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>